<commit_message>
Presentación v2, Memoria terminada
Se han corregido cosas de la presentación haciéndola más liviana. Se han corregido algunos detalles de la memoria.
</commit_message>
<xml_diff>
--- a/Bloque II/parametros.xlsx
+++ b/Bloque II/parametros.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uses0-my.sharepoint.com/personal/joscanege_alum_us_es/Documents/TFG/TFG_GITT_Joscanege/Bloque II/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="727" documentId="13_ncr:1_{DBA3F584-AA4B-469F-8C7C-EB753182C31C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{ADA42EB7-376E-47C6-BA8A-C1501187BF30}"/>
+  <xr:revisionPtr revIDLastSave="728" documentId="13_ncr:1_{DBA3F584-AA4B-469F-8C7C-EB753182C31C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{173487E8-F913-41A8-A7C8-EE08D7DCB9BA}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="4" xr2:uid="{F8534789-7E52-48F9-8D89-E6AD8F7447CD}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="1" xr2:uid="{F8534789-7E52-48F9-8D89-E6AD8F7447CD}"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="5" r:id="rId1"/>
@@ -1698,7 +1698,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1720,10 +1720,10 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2666,13 +2666,7 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{021551F0-3FAA-4A81-816B-7AD3D2172BB0}" name="Tabla1" displayName="Tabla1" ref="A1:J50" totalsRowShown="0" headerRowDxfId="29" dataDxfId="27" headerRowBorderDxfId="28" tableBorderDxfId="26" totalsRowBorderDxfId="25">
-  <autoFilter ref="A1:J50" xr:uid="{021551F0-3FAA-4A81-816B-7AD3D2172BB0}">
-    <filterColumn colId="7">
-      <filters>
-        <filter val="Encuesta"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:J50" xr:uid="{021551F0-3FAA-4A81-816B-7AD3D2172BB0}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A10:J47">
     <sortCondition ref="J1:J50"/>
   </sortState>
@@ -2995,34 +2989,34 @@
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="38" t="s">
+      <c r="A4" s="39" t="s">
         <v>406</v>
       </c>
-      <c r="B4" s="38"/>
-      <c r="C4" s="38"/>
-      <c r="D4" s="38"/>
-      <c r="E4" s="38"/>
-      <c r="F4" s="38"/>
-      <c r="G4" s="38"/>
-      <c r="H4" s="38"/>
-      <c r="I4" s="38"/>
-      <c r="J4" s="38"/>
-      <c r="K4" s="38"/>
-      <c r="L4" s="38"/>
+      <c r="B4" s="39"/>
+      <c r="C4" s="39"/>
+      <c r="D4" s="39"/>
+      <c r="E4" s="39"/>
+      <c r="F4" s="39"/>
+      <c r="G4" s="39"/>
+      <c r="H4" s="39"/>
+      <c r="I4" s="39"/>
+      <c r="J4" s="39"/>
+      <c r="K4" s="39"/>
+      <c r="L4" s="39"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" s="38"/>
-      <c r="B5" s="38"/>
-      <c r="C5" s="38"/>
-      <c r="D5" s="38"/>
-      <c r="E5" s="38"/>
-      <c r="F5" s="38"/>
-      <c r="G5" s="38"/>
-      <c r="H5" s="38"/>
-      <c r="I5" s="38"/>
-      <c r="J5" s="38"/>
-      <c r="K5" s="38"/>
-      <c r="L5" s="38"/>
+      <c r="A5" s="39"/>
+      <c r="B5" s="39"/>
+      <c r="C5" s="39"/>
+      <c r="D5" s="39"/>
+      <c r="E5" s="39"/>
+      <c r="F5" s="39"/>
+      <c r="G5" s="39"/>
+      <c r="H5" s="39"/>
+      <c r="I5" s="39"/>
+      <c r="J5" s="39"/>
+      <c r="K5" s="39"/>
+      <c r="L5" s="39"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
@@ -3030,7 +3024,7 @@
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B8" s="39" t="s">
+      <c r="B8" s="38" t="s">
         <v>407</v>
       </c>
       <c r="D8" t="s">
@@ -3038,7 +3032,7 @@
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B9" s="39" t="s">
+      <c r="B9" s="38" t="s">
         <v>409</v>
       </c>
       <c r="D9" t="s">
@@ -3046,13 +3040,13 @@
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B10" s="39"/>
+      <c r="B10" s="38"/>
       <c r="D10" t="s">
         <v>411</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B11" s="39" t="s">
+      <c r="B11" s="38" t="s">
         <v>413</v>
       </c>
       <c r="D11" t="s">
@@ -3060,7 +3054,7 @@
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B12" s="39" t="s">
+      <c r="B12" s="38" t="s">
         <v>409</v>
       </c>
       <c r="D12" t="s">
@@ -3068,16 +3062,16 @@
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B13" s="39"/>
+      <c r="B13" s="38"/>
       <c r="D13" t="s">
         <v>415</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B14" s="39"/>
+      <c r="B14" s="38"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B15" s="39"/>
+      <c r="B15" s="38"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -3091,7 +3085,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J50"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="N17" sqref="N17"/>
     </sheetView>
   </sheetViews>
@@ -3139,7 +3133,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>10</v>
       </c>
@@ -3172,7 +3166,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>19</v>
       </c>
@@ -3205,7 +3199,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>24</v>
       </c>
@@ -3239,7 +3233,7 @@
         <v>Q76</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>31</v>
       </c>
@@ -3273,7 +3267,7 @@
         <v>Q71</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>35</v>
       </c>
@@ -3307,7 +3301,7 @@
         <v>Q73</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>39</v>
       </c>
@@ -3341,7 +3335,7 @@
         <v>Q72</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>42</v>
       </c>
@@ -3375,7 +3369,7 @@
         <v>Q74</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>45</v>
       </c>
@@ -3477,7 +3471,7 @@
         <v>Q28,Q29</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>60</v>
       </c>
@@ -3681,7 +3675,7 @@
         <v>Q37,Q38</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
         <v>80</v>
       </c>
@@ -3783,7 +3777,7 @@
         <v>Q41,Q42</v>
       </c>
     </row>
-    <row r="21" spans="1:10" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
         <v>89</v>
       </c>
@@ -3885,7 +3879,7 @@
         <v>Q44,Q45</v>
       </c>
     </row>
-    <row r="24" spans="1:10" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
         <v>99</v>
       </c>
@@ -3953,7 +3947,7 @@
         <v>Q46</v>
       </c>
     </row>
-    <row r="26" spans="1:10" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
         <v>105</v>
       </c>
@@ -3987,7 +3981,7 @@
         <v>Q66</v>
       </c>
     </row>
-    <row r="27" spans="1:10" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
         <v>109</v>
       </c>
@@ -4021,7 +4015,7 @@
         <v>Q65</v>
       </c>
     </row>
-    <row r="28" spans="1:10" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
         <v>112</v>
       </c>
@@ -4055,7 +4049,7 @@
         <v>Q69</v>
       </c>
     </row>
-    <row r="29" spans="1:10" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
         <v>115</v>
       </c>
@@ -4089,7 +4083,7 @@
         <v>Q64</v>
       </c>
     </row>
-    <row r="30" spans="1:10" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
         <v>118</v>
       </c>
@@ -4157,7 +4151,7 @@
         <v>Q47,Q48</v>
       </c>
     </row>
-    <row r="32" spans="1:10" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
         <v>128</v>
       </c>
@@ -4191,7 +4185,7 @@
         <v>Q18</v>
       </c>
     </row>
-    <row r="33" spans="1:10" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
         <v>131</v>
       </c>
@@ -4225,7 +4219,7 @@
         <v>Q11,Q12</v>
       </c>
     </row>
-    <row r="34" spans="1:10" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
         <v>136</v>
       </c>
@@ -4259,7 +4253,7 @@
         <v>Q2,Q3</v>
       </c>
     </row>
-    <row r="35" spans="1:10" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
         <v>139</v>
       </c>
@@ -4293,7 +4287,7 @@
         <v>Q13</v>
       </c>
     </row>
-    <row r="36" spans="1:10" ht="50.1" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
         <v>142</v>
       </c>
@@ -4633,7 +4627,7 @@
         <v>Q60</v>
       </c>
     </row>
-    <row r="46" spans="1:10" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A46" s="4" t="s">
         <v>172</v>
       </c>
@@ -4701,7 +4695,7 @@
         <v>Q61,Q62,Q63</v>
       </c>
     </row>
-    <row r="48" spans="1:10" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A48" s="4" t="s">
         <v>178</v>
       </c>
@@ -4735,7 +4729,7 @@
         <v>Q80</v>
       </c>
     </row>
-    <row r="49" spans="1:10" ht="31.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A49" s="4" t="s">
         <v>180</v>
       </c>
@@ -4769,7 +4763,7 @@
         <v>Q82</v>
       </c>
     </row>
-    <row r="50" spans="1:10" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A50" s="4" t="s">
         <v>182</v>
       </c>
@@ -8176,7 +8170,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80894877-A900-4BF4-96DF-F3E83D2156B9}">
   <dimension ref="A1:F156"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E127" sqref="E127"/>
     </sheetView>
   </sheetViews>

</xml_diff>